<commit_message>
added 50 trials for commercial pipette
</commit_message>
<xml_diff>
--- a/data/Reliablity Test 50 Trials 1mL.xlsx
+++ b/data/Reliablity Test 50 Trials 1mL.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fahad\Documents\Git Bash\micropipette\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fahad\Documents\Git Bash\micropipette\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="7005"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="7005" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Pipette" sheetId="1" r:id="rId1"/>
+    <sheet name="Commericial Pipette" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t>Trial</t>
   </si>
@@ -177,7 +178,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$51</c:f>
+              <c:f>'Test Pipette'!$C$2:$C$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -336,7 +337,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$51</c:f>
+              <c:f>'Test Pipette'!$D$2:$D$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -503,11 +504,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1910113536"/>
-        <c:axId val="1864734960"/>
+        <c:axId val="234206656"/>
+        <c:axId val="234195232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1910113536"/>
+        <c:axId val="234206656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -564,12 +565,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1864734960"/>
+        <c:crossAx val="234195232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1864734960"/>
+        <c:axId val="234195232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -626,7 +627,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1910113536"/>
+        <c:crossAx val="234206656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1531,8 +1532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection sqref="A1:D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2192,4 +2193,662 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="52.140625" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0.2024</v>
+      </c>
+      <c r="D2">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>2.6467716594465577E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0.20469999999999999</v>
+      </c>
+      <c r="D3">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.9483019129741338</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>0.2039</v>
+      </c>
+      <c r="D4">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.53672459929969107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>0.2046</v>
+      </c>
+      <c r="D5">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.9245776997255033</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>0.20369999999999999</v>
+      </c>
+      <c r="D6">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.38517382701143299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>0.2044</v>
+      </c>
+      <c r="D7">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.85370321699152318</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>0.20469999999999999</v>
+      </c>
+      <c r="D8">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.9483019129741338</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>0.2044</v>
+      </c>
+      <c r="D9">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.85370321699152318</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="D10">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>5.0889513802385419E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>0.2031</v>
+      </c>
+      <c r="D11">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>7.4336205397422292E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="D12">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.61188602866781583</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>0.2041</v>
+      </c>
+      <c r="D13">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.68306639754315768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>0.2049</v>
+      </c>
+      <c r="D14">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.97792757492818794</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>0.2041</v>
+      </c>
+      <c r="D15">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.68306639754315768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>0.2039</v>
+      </c>
+      <c r="D16">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.53672459929969107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>0.20419999999999999</v>
+      </c>
+      <c r="D17">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.74804284607538918</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>0.20430000000000001</v>
+      </c>
+      <c r="D18">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.8052146928959476</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>0.20380000000000001</v>
+      </c>
+      <c r="D19">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.46022478711426418</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>0.20430000000000001</v>
+      </c>
+      <c r="D20">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.8052146928959476</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>0.20380000000000001</v>
+      </c>
+      <c r="D21">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.46022478711426418</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>0.2039</v>
+      </c>
+      <c r="D22">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.53672459929969107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>0.20380000000000001</v>
+      </c>
+      <c r="D23">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.46022478711426418</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>0.2036</v>
+      </c>
+      <c r="D24">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.31420254053967234</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>0.2041</v>
+      </c>
+      <c r="D25">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.68306639754315768</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>0.20319999999999999</v>
+      </c>
+      <c r="D26">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.10525142539243772</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>0.20269999999999999</v>
+      </c>
+      <c r="D27">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>1.346787383407707E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>0.2039</v>
+      </c>
+      <c r="D28">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.53672459929969107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="D29">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.61188602866781583</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>0.2031</v>
+      </c>
+      <c r="D30">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>7.4336205397422292E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>0.20419999999999999</v>
+      </c>
+      <c r="D31">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.74804284607538918</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <v>0.2039</v>
+      </c>
+      <c r="D32">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.53672459929969107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>0.20380000000000001</v>
+      </c>
+      <c r="D33">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.46022478711426418</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>0.2036</v>
+      </c>
+      <c r="D34">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.31420254053967234</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>0.2046</v>
+      </c>
+      <c r="D35">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.9245776997255033</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>0.2034</v>
+      </c>
+      <c r="D36">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.19267569947363233</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <v>0.20319999999999999</v>
+      </c>
+      <c r="D37">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.10525142539243772</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <v>0.20369999999999999</v>
+      </c>
+      <c r="D38">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.38517382701143299</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <v>0.2034</v>
+      </c>
+      <c r="D39">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.19267569947363233</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <v>0.2034</v>
+      </c>
+      <c r="D40">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.19267569947363233</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <v>0.20419999999999999</v>
+      </c>
+      <c r="D41">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.74804284607538918</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <v>0.2041</v>
+      </c>
+      <c r="D42">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.68306639754315768</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="C43">
+        <v>0.2039</v>
+      </c>
+      <c r="D43">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.53672459929969107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="C44">
+        <v>0.20380000000000001</v>
+      </c>
+      <c r="D44">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.46022478711426418</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="C45">
+        <v>0.2034</v>
+      </c>
+      <c r="D45">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.19267569947363233</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="C46">
+        <v>0.20449999999999999</v>
+      </c>
+      <c r="D46">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.89334253477604819</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="C47">
+        <v>0.20330000000000001</v>
+      </c>
+      <c r="D47">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.14454246253646461</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="C48">
+        <v>0.2039</v>
+      </c>
+      <c r="D48">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.53672459929969107</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="C49">
+        <v>0.20369999999999999</v>
+      </c>
+      <c r="D49">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.38517382701143299</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>0.2041</v>
+      </c>
+      <c r="D50">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.68306639754315768</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="C51">
+        <v>0.2039</v>
+      </c>
+      <c r="D51">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.53672459929969107</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54">
+        <f>AVERAGE(C2:C51)</f>
+        <v>0.20385200000000009</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55">
+        <f>STDEV(C2:C51)</f>
+        <v>5.2069027967395216E-4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56">
+        <f>(C55/(SQRT(50)))</f>
+        <v>7.3636725531074304E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>